<commit_message>
Modificacion de Script para carga de datos desde excel
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\Mascota\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E51B7A-3F49-4131-8D4F-15715F5F499C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Compras" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Compras!$A$1:$L$999</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="sCtyU1WbGnyjYrVJChugRqMiHc2nOVszYKXBn/oAtDw="/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="290">
   <si>
     <t>Mes</t>
   </si>
@@ -894,21 +893,40 @@
   <si>
     <t>Holmberg</t>
   </si>
+  <si>
+    <t>de prueba</t>
+  </si>
+  <si>
+    <t>deprueba</t>
+  </si>
+  <si>
+    <t>* prueba</t>
+  </si>
+  <si>
+    <t>12 Prueba</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@"/>
     <numFmt numFmtId="165" formatCode="[$USD]\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="00000000000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1148,134 +1166,135 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1490,7 +1509,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -34657,8 +34676,8 @@
       <c r="K1000" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L999" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L166">
+  <autoFilter ref="A1:L999"/>
+  <sortState ref="A2:L166">
     <sortCondition ref="B2:B166"/>
     <sortCondition ref="A2:A166"/>
   </sortState>
@@ -34668,12 +34687,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="C73" sqref="C2:C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -46148,12 +46167,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED89AD41-FB27-43E8-A8DE-77DC0372D815}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -46226,7 +46245,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A73">
+  <sortState ref="A2:A73">
     <sortCondition ref="A2:A73"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -46234,11 +46253,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A671D3C-078A-4850-B4D8-DB6CB402A869}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -46310,16 +46329,57 @@
         <v>30503508725</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="48" t="s">
+        <v>287</v>
+      </c>
+      <c r="B9" s="49">
+        <v>30503508725</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="48" t="s">
+        <v>286</v>
+      </c>
+      <c r="B10" s="49">
+        <v>30503508725</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="48" t="s">
+        <v>288</v>
+      </c>
+      <c r="B11" s="49">
+        <v>30503508725</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="B12" s="49">
+        <v>30503508725</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="49">
+        <v>30503508725</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A22">
+  <sortState ref="A2:A22">
     <sortCondition ref="A2:A22"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -51510,7 +51570,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EB15C8-E537-449B-AC50-3D74D04675C3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -51561,7 +51621,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -62115,7 +62175,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Correcion en script para carga de proveedores
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\Mascota\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B007FA6-FCED-4A0C-8F7C-4894D1D4ABC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compras" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Compras!$A$1:$L$999</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="sCtyU1WbGnyjYrVJChugRqMiHc2nOVszYKXBn/oAtDw="/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="286">
   <si>
     <t>Mes</t>
   </si>
@@ -893,40 +894,21 @@
   <si>
     <t>Holmberg</t>
   </si>
-  <si>
-    <t>de prueba</t>
-  </si>
-  <si>
-    <t>deprueba</t>
-  </si>
-  <si>
-    <t>* prueba</t>
-  </si>
-  <si>
-    <t>12 Prueba</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@"/>
     <numFmt numFmtId="165" formatCode="[$USD]\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="00000000000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1166,135 +1148,134 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1509,7 +1490,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -34676,8 +34657,8 @@
       <c r="K1000" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L999"/>
-  <sortState ref="A2:L166">
+  <autoFilter ref="A1:L999" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L166">
     <sortCondition ref="B2:B166"/>
     <sortCondition ref="A2:A166"/>
   </sortState>
@@ -34687,10 +34668,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C73" sqref="C2:C73"/>
     </sheetView>
@@ -46172,7 +46153,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -46245,7 +46226,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:A73">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A73">
     <sortCondition ref="A2:A73"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -46253,11 +46234,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -46331,47 +46312,15 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="48" t="s">
-        <v>287</v>
-      </c>
-      <c r="B9" s="49">
-        <v>30503508725</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="48" t="s">
-        <v>286</v>
-      </c>
-      <c r="B10" s="49">
-        <v>30503508725</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="48" t="s">
-        <v>288</v>
-      </c>
-      <c r="B11" s="49">
-        <v>30503508725</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="48" t="s">
-        <v>289</v>
-      </c>
-      <c r="B12" s="49">
-        <v>30503508725</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="B13" s="49">
-        <v>30503508725</v>
+      <c r="B9" s="44">
+        <v>33502232229</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:A22">
-    <sortCondition ref="A2:A22"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A18">
+    <sortCondition ref="A2:A18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -46379,7 +46328,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -51570,7 +51519,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -51621,7 +51570,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -62175,7 +62124,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>